<commit_message>
fixed problem with mapper and app is now saving stats to db
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -47,37 +47,37 @@
     <t>Lundo’s Legends</t>
   </si>
   <si>
+    <t>EL Onće</t>
+  </si>
+  <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
     <t>Samsquanches</t>
   </si>
   <si>
     <t>Epic7</t>
   </si>
   <si>
-    <t>EL Onće</t>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>Splitfinger Skadoosh</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>MillerTime</t>
   </si>
   <si>
     <t>SmokeWalkers</t>
   </si>
   <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
-    <t>MillerTime</t>
-  </si>
-  <si>
-    <t>GOD WILLS IT</t>
-  </si>
-  <si>
-    <t>Splitfinger Skadoosh</t>
-  </si>
-  <si>
-    <t>Swampnuts</t>
-  </si>
-  <si>
     <t>Mac</t>
-  </si>
-  <si>
-    <t>confusion</t>
   </si>
   <si>
     <t>DJ's Quality Team</t>
@@ -180,23 +180,23 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>124.5</v>
+        <v>139.5</v>
       </c>
       <c r="D2" t="n">
-        <v>60.5</v>
+        <v>62.5</v>
       </c>
       <c r="E2" t="n">
-        <v>64.0</v>
+        <v>77.0</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>-15.0</v>
+        <v>15.0</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.0</v>
+        <v>2.0</v>
       </c>
       <c r="I2" t="n">
-        <v>-13.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="3">
@@ -207,23 +207,23 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>98.0</v>
+        <v>124.5</v>
       </c>
       <c r="D3" t="n">
-        <v>56.0</v>
+        <v>60.5</v>
       </c>
       <c r="E3" t="n">
-        <v>42.0</v>
+        <v>64.0</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>-5.5</v>
+        <v>34.0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="I3" t="n">
-        <v>-5.5</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="4">
@@ -234,23 +234,23 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>91.0</v>
+        <v>107.0</v>
       </c>
       <c r="D4" t="n">
         <v>45.0</v>
       </c>
       <c r="E4" t="n">
-        <v>46.0</v>
+        <v>62.0</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>-5.0</v>
+        <v>20.5</v>
       </c>
       <c r="H4" t="n">
-        <v>7.0</v>
+        <v>9.5</v>
       </c>
       <c r="I4" t="n">
-        <v>-12.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="5">
@@ -261,23 +261,23 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>90.5</v>
+        <v>103.5</v>
       </c>
       <c r="D5" t="n">
-        <v>40.5</v>
+        <v>56.0</v>
       </c>
       <c r="E5" t="n">
-        <v>50.0</v>
+        <v>47.5</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>-34.0</v>
+        <v>5.5</v>
       </c>
       <c r="H5" t="n">
-        <v>-20.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>-14.0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6">
@@ -288,104 +288,104 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>88.5</v>
+        <v>96.0</v>
       </c>
       <c r="D6" t="n">
-        <v>62.5</v>
+        <v>38.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>58.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>14.0</v>
+        <v>5.0</v>
       </c>
       <c r="H6" t="n">
-        <v>23.0</v>
+        <v>-7.0</v>
       </c>
       <c r="I6" t="n">
-        <v>-9.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.0</v>
+        <v>6.5</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>86.5</v>
+        <v>89.5</v>
       </c>
       <c r="D7" t="n">
-        <v>35.5</v>
+        <v>47.5</v>
       </c>
       <c r="E7" t="n">
-        <v>51.0</v>
+        <v>42.0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>-20.5</v>
+        <v>5.5</v>
       </c>
       <c r="H7" t="n">
-        <v>-9.5</v>
+        <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>-11.0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>84.0</v>
+        <v>89.5</v>
       </c>
       <c r="D8" t="n">
-        <v>49.5</v>
+        <v>35.5</v>
       </c>
       <c r="E8" t="n">
-        <v>34.5</v>
+        <v>54.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="H8" t="n">
-        <v>11.0</v>
+        <v>-4.0</v>
       </c>
       <c r="I8" t="n">
-        <v>-3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7.5</v>
+        <v>8.0</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>84.0</v>
+        <v>81.5</v>
       </c>
       <c r="D9" t="n">
-        <v>47.5</v>
+        <v>49.5</v>
       </c>
       <c r="E9" t="n">
-        <v>36.5</v>
+        <v>32.0</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>-5.5</v>
+        <v>12.5</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0</v>
+        <v>11.5</v>
       </c>
       <c r="I9" t="n">
-        <v>-5.5</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -396,23 +396,23 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>83.5</v>
+        <v>79.0</v>
       </c>
       <c r="D10" t="n">
-        <v>39.5</v>
+        <v>35.5</v>
       </c>
       <c r="E10" t="n">
-        <v>44.0</v>
+        <v>43.5</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>-6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H10" t="n">
-        <v>4.0</v>
+        <v>-3.0</v>
       </c>
       <c r="I10" t="n">
-        <v>-10.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
@@ -423,23 +423,23 @@
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>74.0</v>
+        <v>76.0</v>
       </c>
       <c r="D11" t="n">
         <v>38.5</v>
       </c>
       <c r="E11" t="n">
-        <v>35.5</v>
+        <v>37.5</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>-5.0</v>
+        <v>-8.0</v>
       </c>
       <c r="H11" t="n">
+        <v>-11.0</v>
+      </c>
+      <c r="I11" t="n">
         <v>3.0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-8.0</v>
       </c>
     </row>
     <row r="12">
@@ -450,23 +450,23 @@
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>69.5</v>
+        <v>74.5</v>
       </c>
       <c r="D12" t="n">
-        <v>35.5</v>
+        <v>39.5</v>
       </c>
       <c r="E12" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>-4.5</v>
+        <v>-14.0</v>
       </c>
       <c r="H12" t="n">
-        <v>-2.5</v>
+        <v>-23.0</v>
       </c>
       <c r="I12" t="n">
-        <v>-2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="13">
@@ -477,23 +477,23 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>69.0</v>
+        <v>74.0</v>
       </c>
       <c r="D13" t="n">
         <v>38.0</v>
       </c>
       <c r="E13" t="n">
-        <v>31.0</v>
+        <v>36.0</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>-12.5</v>
+        <v>4.5</v>
       </c>
       <c r="H13" t="n">
-        <v>-11.5</v>
+        <v>2.5</v>
       </c>
       <c r="I13" t="n">
-        <v>-1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
@@ -504,23 +504,23 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>56.5</v>
+        <v>64.5</v>
       </c>
       <c r="D14" t="n">
-        <v>38.0</v>
+        <v>40.5</v>
       </c>
       <c r="E14" t="n">
-        <v>18.5</v>
+        <v>24.0</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>-8.0</v>
+        <v>8.0</v>
       </c>
       <c r="H14" t="n">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
       <c r="I14" t="n">
-        <v>-5.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="15">
@@ -531,23 +531,23 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>55.5</v>
+        <v>61.0</v>
       </c>
       <c r="D15" t="n">
         <v>43.5</v>
       </c>
       <c r="E15" t="n">
-        <v>12.0</v>
+        <v>17.5</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>-5.5</v>
+        <v>5.5</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>-5.5</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving before I refactor flow of pojos
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -190,13 +190,13 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -217,13 +217,13 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -244,13 +244,13 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>20.5</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
-        <v>9.5</v>
+        <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -271,13 +271,13 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -298,13 +298,13 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>-7.0</v>
+        <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -325,13 +325,13 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -352,13 +352,13 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>-4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I8" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -379,13 +379,13 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>12.5</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>11.5</v>
+        <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -406,13 +406,13 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H10" t="n">
-        <v>-3.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -433,13 +433,13 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>-8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="n">
-        <v>-11.0</v>
+        <v>0.0</v>
       </c>
       <c r="I11" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -460,13 +460,13 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>-14.0</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
-        <v>-23.0</v>
+        <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -487,13 +487,13 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>4.5</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n">
-        <v>2.5</v>
+        <v>0.0</v>
       </c>
       <c r="I13" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -514,13 +514,13 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
-        <v>2.5</v>
+        <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -541,13 +541,13 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>5.5</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reworked service to map to Stats, calculate, save, and then map to Roto and also fixed excel writer to have space
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -29,7 +29,7 @@
     <t>pitching</t>
   </si>
   <si>
-    <t>__</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>total_change</t>
@@ -56,34 +56,34 @@
     <t>Samsquanches</t>
   </si>
   <si>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>Splitfinger Skadoosh</t>
+  </si>
+  <si>
     <t>Epic7</t>
   </si>
   <si>
-    <t>GOD WILLS IT</t>
-  </si>
-  <si>
-    <t>Splitfinger Skadoosh</t>
+    <t>MillerTime</t>
   </si>
   <si>
     <t>confusion</t>
   </si>
   <si>
-    <t>Swampnuts</t>
-  </si>
-  <si>
-    <t>MillerTime</t>
-  </si>
-  <si>
     <t>SmokeWalkers</t>
   </si>
   <si>
     <t>Mac</t>
   </si>
   <si>
+    <t>Corbin Copy</t>
+  </si>
+  <si>
     <t>DJ's Quality Team</t>
-  </si>
-  <si>
-    <t>Corbin Copy</t>
   </si>
 </sst>
 </file>
@@ -180,13 +180,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>139.5</v>
+        <v>133.0</v>
       </c>
       <c r="D2" t="n">
-        <v>62.5</v>
+        <v>60.0</v>
       </c>
       <c r="E2" t="n">
-        <v>77.0</v>
+        <v>73.0</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
@@ -207,13 +207,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>124.5</v>
+        <v>124.0</v>
       </c>
       <c r="D3" t="n">
-        <v>60.5</v>
+        <v>58.0</v>
       </c>
       <c r="E3" t="n">
-        <v>64.0</v>
+        <v>66.0</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
@@ -234,13 +234,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>107.0</v>
+        <v>114.0</v>
       </c>
       <c r="D4" t="n">
-        <v>45.0</v>
+        <v>56.0</v>
       </c>
       <c r="E4" t="n">
-        <v>62.0</v>
+        <v>58.0</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
@@ -261,13 +261,13 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>103.5</v>
+        <v>99.0</v>
       </c>
       <c r="D5" t="n">
-        <v>56.0</v>
+        <v>53.0</v>
       </c>
       <c r="E5" t="n">
-        <v>47.5</v>
+        <v>46.0</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
@@ -288,13 +288,13 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>96.0</v>
+        <v>97.0</v>
       </c>
       <c r="D6" t="n">
-        <v>38.0</v>
+        <v>46.0</v>
       </c>
       <c r="E6" t="n">
-        <v>58.0</v>
+        <v>51.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
@@ -309,19 +309,19 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.5</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>89.5</v>
+        <v>89.0</v>
       </c>
       <c r="D7" t="n">
-        <v>47.5</v>
+        <v>33.0</v>
       </c>
       <c r="E7" t="n">
-        <v>42.0</v>
+        <v>56.0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
@@ -336,16 +336,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6.5</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>89.5</v>
+        <v>88.0</v>
       </c>
       <c r="D8" t="n">
-        <v>35.5</v>
+        <v>34.0</v>
       </c>
       <c r="E8" t="n">
         <v>54.0</v>
@@ -369,13 +369,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>81.5</v>
+        <v>83.0</v>
       </c>
       <c r="D9" t="n">
-        <v>49.5</v>
+        <v>36.0</v>
       </c>
       <c r="E9" t="n">
-        <v>32.0</v>
+        <v>47.0</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
@@ -396,13 +396,13 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>79.0</v>
+        <v>78.0</v>
       </c>
       <c r="D10" t="n">
-        <v>35.5</v>
+        <v>44.0</v>
       </c>
       <c r="E10" t="n">
-        <v>43.5</v>
+        <v>34.0</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
@@ -417,19 +417,19 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10.0</v>
+        <v>10.5</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>76.0</v>
+        <v>72.0</v>
       </c>
       <c r="D11" t="n">
-        <v>38.5</v>
+        <v>47.0</v>
       </c>
       <c r="E11" t="n">
-        <v>37.5</v>
+        <v>25.0</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
@@ -444,16 +444,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11.0</v>
+        <v>10.5</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>74.5</v>
+        <v>72.0</v>
       </c>
       <c r="D12" t="n">
-        <v>39.5</v>
+        <v>37.0</v>
       </c>
       <c r="E12" t="n">
         <v>35.0</v>
@@ -477,13 +477,13 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>74.0</v>
+        <v>67.0</v>
       </c>
       <c r="D13" t="n">
-        <v>38.0</v>
+        <v>36.0</v>
       </c>
       <c r="E13" t="n">
-        <v>36.0</v>
+        <v>31.0</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
@@ -504,13 +504,13 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>64.5</v>
+        <v>64.0</v>
       </c>
       <c r="D14" t="n">
-        <v>40.5</v>
+        <v>43.0</v>
       </c>
       <c r="E14" t="n">
-        <v>24.0</v>
+        <v>21.0</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
@@ -531,13 +531,13 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="D15" t="n">
-        <v>43.5</v>
+        <v>40.0</v>
       </c>
       <c r="E15" t="n">
-        <v>17.5</v>
+        <v>22.0</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">

</xml_diff>

<commit_message>
added ranks and condensed excel logic
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>rank</t>
   </si>
@@ -44,15 +44,15 @@
     <t/>
   </si>
   <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
     <t>Lundo’s Legends</t>
   </si>
   <si>
     <t>EL Onće</t>
   </si>
   <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
     <t>Samsquanches</t>
   </si>
   <si>
@@ -62,28 +62,31 @@
     <t>Swampnuts</t>
   </si>
   <si>
+    <t>MillerTime</t>
+  </si>
+  <si>
+    <t>Epic7</t>
+  </si>
+  <si>
     <t>Splitfinger Skadoosh</t>
   </si>
   <si>
-    <t>Epic7</t>
-  </si>
-  <si>
-    <t>MillerTime</t>
+    <t>DJ's Quality Team</t>
+  </si>
+  <si>
+    <t>Corbin Copy</t>
+  </si>
+  <si>
+    <t>SmokeWalkers</t>
   </si>
   <si>
     <t>confusion</t>
   </si>
   <si>
-    <t>SmokeWalkers</t>
-  </si>
-  <si>
     <t>Mac</t>
   </si>
   <si>
-    <t>Corbin Copy</t>
-  </si>
-  <si>
-    <t>DJ's Quality Team</t>
+    <t xml:space="preserve">name </t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,20 +183,20 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>133.0</v>
+        <v>138.0</v>
       </c>
       <c r="D2" t="n">
-        <v>60.0</v>
+        <v>82.0</v>
       </c>
       <c r="E2" t="n">
-        <v>73.0</v>
+        <v>56.0</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I2" t="n">
         <v>0.0</v>
@@ -207,23 +210,23 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>124.0</v>
+        <v>121.0</v>
       </c>
       <c r="D3" t="n">
         <v>58.0</v>
       </c>
       <c r="E3" t="n">
-        <v>66.0</v>
+        <v>63.0</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -234,23 +237,23 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>114.0</v>
+        <v>111.0</v>
       </c>
       <c r="D4" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
       <c r="E4" t="n">
-        <v>58.0</v>
+        <v>54.0</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>-10.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>-10.0</v>
       </c>
     </row>
     <row r="5">
@@ -261,10 +264,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>99.0</v>
+        <v>96.0</v>
       </c>
       <c r="D5" t="n">
-        <v>53.0</v>
+        <v>50.0</v>
       </c>
       <c r="E5" t="n">
         <v>46.0</v>
@@ -274,10 +277,10 @@
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -288,20 +291,20 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>97.0</v>
+        <v>93.0</v>
       </c>
       <c r="D6" t="n">
-        <v>46.0</v>
+        <v>39.0</v>
       </c>
       <c r="E6" t="n">
-        <v>51.0</v>
+        <v>54.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
@@ -315,13 +318,13 @@
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>89.0</v>
+        <v>88.0</v>
       </c>
       <c r="D7" t="n">
         <v>33.0</v>
       </c>
       <c r="E7" t="n">
-        <v>56.0</v>
+        <v>55.0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
@@ -342,23 +345,23 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>88.0</v>
+        <v>85.0</v>
       </c>
       <c r="D8" t="n">
-        <v>34.0</v>
+        <v>42.0</v>
       </c>
       <c r="E8" t="n">
-        <v>54.0</v>
+        <v>43.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="9">
@@ -369,20 +372,20 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>83.0</v>
+        <v>81.0</v>
       </c>
       <c r="D9" t="n">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="E9" t="n">
         <v>47.0</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I9" t="n">
         <v>0.0</v>
@@ -399,10 +402,10 @@
         <v>78.0</v>
       </c>
       <c r="D10" t="n">
-        <v>44.0</v>
+        <v>32.0</v>
       </c>
       <c r="E10" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
@@ -423,13 +426,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
       <c r="D11" t="n">
-        <v>47.0</v>
+        <v>40.0</v>
       </c>
       <c r="E11" t="n">
-        <v>25.0</v>
+        <v>33.0</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
@@ -450,23 +453,23 @@
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>72.0</v>
+        <v>73.0</v>
       </c>
       <c r="D12" t="n">
-        <v>37.0</v>
+        <v>42.0</v>
       </c>
       <c r="E12" t="n">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="H12" t="n">
         <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="13">
@@ -477,23 +480,23 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>67.0</v>
+        <v>71.0</v>
       </c>
       <c r="D13" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="E13" t="n">
         <v>36.0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>31.0</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
         <v>0.0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="14">
@@ -504,23 +507,23 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>64.0</v>
+        <v>69.0</v>
       </c>
       <c r="D14" t="n">
-        <v>43.0</v>
+        <v>45.0</v>
       </c>
       <c r="E14" t="n">
-        <v>21.0</v>
+        <v>24.0</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="15">
@@ -531,23 +534,297 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>62.0</v>
+        <v>68.0</v>
       </c>
       <c r="D15" t="n">
-        <v>40.0</v>
+        <v>34.0</v>
       </c>
       <c r="E15" t="n">
-        <v>22.0</v>
+        <v>34.0</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
         <v>0.0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="n">
+        <v>63.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="n">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="n">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="n">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="n">
+        <v>47.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="n">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="n">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="n">
+        <v>43.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="n">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="n">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="n">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" t="n">
+        <v>24.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added exact rank to each category and improved tie method
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
   <si>
     <t>rank</t>
   </si>
@@ -32,13 +32,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>total_change</t>
-  </si>
-  <si>
-    <t>hitting_change</t>
-  </si>
-  <si>
-    <t>pitching_change</t>
+    <t>total change</t>
+  </si>
+  <si>
+    <t>hitting change</t>
+  </si>
+  <si>
+    <t>pitching change</t>
   </si>
   <si>
     <t/>
@@ -59,12 +59,12 @@
     <t>GOD WILLS IT</t>
   </si>
   <si>
+    <t>MillerTime</t>
+  </si>
+  <si>
     <t>Swampnuts</t>
   </si>
   <si>
-    <t>MillerTime</t>
-  </si>
-  <si>
     <t>Epic7</t>
   </si>
   <si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rank </t>
   </si>
   <si>
     <t xml:space="preserve">name </t>
@@ -183,20 +186,20 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>138.0</v>
+        <v>137.5</v>
       </c>
       <c r="D2" t="n">
-        <v>82.0</v>
+        <v>81.5</v>
       </c>
       <c r="E2" t="n">
         <v>56.0</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n">
         <v>0.0</v>
@@ -210,10 +213,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>121.0</v>
+        <v>120.5</v>
       </c>
       <c r="D3" t="n">
-        <v>58.0</v>
+        <v>57.5</v>
       </c>
       <c r="E3" t="n">
         <v>63.0</v>
@@ -223,10 +226,10 @@
         <v>0.0</v>
       </c>
       <c r="H3" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -237,23 +240,23 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>111.0</v>
+        <v>112.0</v>
       </c>
       <c r="D4" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="E4" t="n">
         <v>54.0</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>-10.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>-10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -277,10 +280,10 @@
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -291,20 +294,20 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>93.0</v>
+        <v>93.5</v>
       </c>
       <c r="D6" t="n">
-        <v>39.0</v>
+        <v>39.5</v>
       </c>
       <c r="E6" t="n">
         <v>54.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
@@ -318,13 +321,13 @@
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>88.0</v>
+        <v>91.5</v>
       </c>
       <c r="D7" t="n">
-        <v>33.0</v>
+        <v>48.5</v>
       </c>
       <c r="E7" t="n">
-        <v>55.0</v>
+        <v>43.0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
@@ -345,23 +348,23 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>85.0</v>
+        <v>87.5</v>
       </c>
       <c r="D8" t="n">
-        <v>42.0</v>
+        <v>32.5</v>
       </c>
       <c r="E8" t="n">
-        <v>43.0</v>
+        <v>55.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>-2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I8" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -372,20 +375,20 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>81.0</v>
+        <v>84.5</v>
       </c>
       <c r="D9" t="n">
-        <v>34.0</v>
+        <v>35.5</v>
       </c>
       <c r="E9" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I9" t="n">
         <v>0.0</v>
@@ -399,13 +402,13 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>78.0</v>
+        <v>79.0</v>
       </c>
       <c r="D10" t="n">
         <v>32.0</v>
       </c>
       <c r="E10" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
@@ -420,19 +423,19 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10.5</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>73.0</v>
+        <v>74.5</v>
       </c>
       <c r="D11" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="E11" t="n">
-        <v>33.0</v>
+        <v>33.5</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
@@ -447,29 +450,29 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10.5</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>73.0</v>
+        <v>73.5</v>
       </c>
       <c r="D12" t="n">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="E12" t="n">
-        <v>31.0</v>
+        <v>32.5</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
         <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -483,20 +486,20 @@
         <v>71.0</v>
       </c>
       <c r="D13" t="n">
-        <v>35.0</v>
+        <v>34.5</v>
       </c>
       <c r="E13" t="n">
-        <v>36.0</v>
+        <v>36.5</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
         <v>0.0</v>
       </c>
       <c r="H13" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -507,23 +510,23 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>69.0</v>
+        <v>70.5</v>
       </c>
       <c r="D14" t="n">
-        <v>45.0</v>
+        <v>45.5</v>
       </c>
       <c r="E14" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -534,23 +537,23 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>68.0</v>
+        <v>68.5</v>
       </c>
       <c r="D15" t="n">
-        <v>34.0</v>
+        <v>33.0</v>
       </c>
       <c r="E15" t="n">
-        <v>34.0</v>
+        <v>35.5</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
         <v>0.0</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16"/>
@@ -572,6 +575,9 @@
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -583,13 +589,16 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>82.0</v>
+        <v>81.5</v>
       </c>
       <c r="D19"/>
-      <c r="E19" t="s">
+      <c r="E19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>63.0</v>
       </c>
     </row>
@@ -598,16 +607,19 @@
         <v>2.0</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
         <v>58.0</v>
       </c>
       <c r="D20"/>
-      <c r="E20" t="s">
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>56.0</v>
       </c>
     </row>
@@ -616,16 +628,19 @@
         <v>3.0</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>57.0</v>
+        <v>57.5</v>
       </c>
       <c r="D21"/>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="n">
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="n">
         <v>55.0</v>
       </c>
     </row>
@@ -640,10 +655,13 @@
         <v>50.0</v>
       </c>
       <c r="D22"/>
-      <c r="E22" t="s">
+      <c r="E22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F22" t="s">
         <v>12</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>54.0</v>
       </c>
     </row>
@@ -652,16 +670,19 @@
         <v>5.0</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C23" t="n">
-        <v>45.0</v>
+        <v>48.5</v>
       </c>
       <c r="D23"/>
-      <c r="E23" t="s">
+      <c r="E23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F23" t="s">
         <v>14</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>54.0</v>
       </c>
     </row>
@@ -670,52 +691,61 @@
         <v>6.0</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>42.0</v>
+        <v>45.5</v>
       </c>
       <c r="D24"/>
-      <c r="E24" t="s">
+      <c r="E24" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="n">
-        <v>47.0</v>
+      <c r="G24" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="n">
         <v>7.0</v>
       </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="D25"/>
-      <c r="E25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" t="n">
-        <v>46.0</v>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" t="n">
         <v>8.0</v>
       </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="D26"/>
-      <c r="E26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="n">
         <v>46.0</v>
       </c>
     </row>
@@ -727,13 +757,16 @@
         <v>14</v>
       </c>
       <c r="C27" t="n">
-        <v>39.0</v>
+        <v>39.5</v>
       </c>
       <c r="D27"/>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="E27" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" t="n">
         <v>43.0</v>
       </c>
     </row>
@@ -742,17 +775,20 @@
         <v>10.0</v>
       </c>
       <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F28" t="s">
         <v>21</v>
       </c>
-      <c r="C28" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="n">
-        <v>36.0</v>
+      <c r="G28" t="n">
+        <v>36.5</v>
       </c>
     </row>
     <row r="29">
@@ -760,17 +796,20 @@
         <v>11.0</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" t="n">
-        <v>34.0</v>
+        <v>34.5</v>
       </c>
       <c r="D29"/>
-      <c r="E29" t="s">
+      <c r="E29" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="F29" t="n">
-        <v>34.0</v>
+      <c r="G29" t="n">
+        <v>35.5</v>
       </c>
     </row>
     <row r="30">
@@ -781,14 +820,17 @@
         <v>23</v>
       </c>
       <c r="C30" t="n">
-        <v>34.0</v>
+        <v>33.0</v>
       </c>
       <c r="D30"/>
-      <c r="E30" t="s">
+      <c r="E30" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F30" t="s">
         <v>19</v>
       </c>
-      <c r="F30" t="n">
-        <v>33.0</v>
+      <c r="G30" t="n">
+        <v>33.5</v>
       </c>
     </row>
     <row r="31">
@@ -796,17 +838,20 @@
         <v>13.0</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31" t="n">
-        <v>33.0</v>
+        <v>32.5</v>
       </c>
       <c r="D31"/>
-      <c r="E31" t="s">
+      <c r="E31" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="F31" t="s">
         <v>20</v>
       </c>
-      <c r="F31" t="n">
-        <v>31.0</v>
+      <c r="G31" t="n">
+        <v>32.5</v>
       </c>
     </row>
     <row r="32">
@@ -820,11 +865,14 @@
         <v>32.0</v>
       </c>
       <c r="D32"/>
-      <c r="E32" t="s">
+      <c r="E32" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="F32" t="s">
         <v>22</v>
       </c>
-      <c r="F32" t="n">
-        <v>24.0</v>
+      <c r="G32" t="n">
+        <v>25.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved placement of change calculations and replacing magic numbers with enums
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results.xlsx
+++ b/src/main/resources/files/results.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" r:id="rId3" sheetId="1"/>
+    <sheet name="LastMonth" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="26">
   <si>
     <t>rank</t>
   </si>
@@ -143,7 +144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -202,7 +203,7 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>-56.0</v>
       </c>
     </row>
     <row r="3">
@@ -229,7 +230,7 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>-63.0</v>
       </c>
     </row>
     <row r="4">
@@ -256,7 +257,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>-54.0</v>
       </c>
     </row>
     <row r="5">
@@ -283,7 +284,7 @@
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0</v>
+        <v>-46.0</v>
       </c>
     </row>
     <row r="6">
@@ -310,7 +311,7 @@
         <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0</v>
+        <v>-54.0</v>
       </c>
     </row>
     <row r="7">
@@ -337,7 +338,7 @@
         <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0</v>
+        <v>-43.0</v>
       </c>
     </row>
     <row r="8">
@@ -364,7 +365,7 @@
         <v>0.0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0</v>
+        <v>-55.0</v>
       </c>
     </row>
     <row r="9">
@@ -391,7 +392,7 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0</v>
+        <v>-49.0</v>
       </c>
     </row>
     <row r="10">
@@ -418,7 +419,7 @@
         <v>0.0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0</v>
+        <v>-47.0</v>
       </c>
     </row>
     <row r="11">
@@ -445,7 +446,7 @@
         <v>0.0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0</v>
+        <v>-33.5</v>
       </c>
     </row>
     <row r="12">
@@ -472,7 +473,7 @@
         <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0</v>
+        <v>-32.5</v>
       </c>
     </row>
     <row r="13">
@@ -499,7 +500,7 @@
         <v>0.0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0</v>
+        <v>-36.5</v>
       </c>
     </row>
     <row r="14">
@@ -526,7 +527,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0</v>
+        <v>-25.0</v>
       </c>
     </row>
     <row r="15">
@@ -553,113 +554,133 @@
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>-35.5</v>
       </c>
     </row>
     <row r="16"/>
-    <row r="17"/>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>4</v>
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="n">
+        <v>63.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>81.5</v>
+        <v>58.0</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>63.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="n">
-        <v>58.0</v>
+        <v>57.5</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G20" t="n">
-        <v>56.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>57.5</v>
+        <v>50.0</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="n">
-        <v>3.0</v>
+        <v>4.5</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G21" t="n">
-        <v>55.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C22" t="n">
-        <v>50.0</v>
+        <v>48.5</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="n">
         <v>4.5</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G22" t="n">
         <v>54.0</v>
@@ -667,44 +688,44 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>48.5</v>
+        <v>45.5</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="n">
-        <v>4.5</v>
+        <v>6.0</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G23" t="n">
-        <v>54.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>6.0</v>
+        <v>7.5</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>45.5</v>
+        <v>41.0</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G24" t="n">
-        <v>49.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="25">
@@ -712,167 +733,582 @@
         <v>7.5</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C25" t="n">
         <v>41.0</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G25" t="n">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>7.5</v>
+        <v>9.0</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
-        <v>41.0</v>
+        <v>39.5</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G26" t="n">
-        <v>46.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C27" t="n">
-        <v>39.5</v>
+        <v>35.5</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G27" t="n">
-        <v>43.0</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C28" t="n">
-        <v>35.5</v>
+        <v>34.5</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C29" t="n">
-        <v>34.5</v>
+        <v>33.0</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G29" t="n">
-        <v>35.5</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C30" t="n">
-        <v>33.0</v>
+        <v>32.5</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" t="n">
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C31" t="n">
-        <v>32.5</v>
+        <v>32.0</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="n">
+        <v>25.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="n">
+        <v>94.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="n">
+        <v>94.5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="n">
+        <v>85.5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
         <v>13.0</v>
       </c>
-      <c r="F31" t="s">
-        <v>20</v>
-      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30" t="n">
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F31"/>
       <c r="G31" t="n">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="D32"/>
-      <c r="E32" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" t="n">
-        <v>25.0</v>
+        <v>0.10999999940395355</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>